<commit_message>
First suspend operation is running. TC02: Idle is periodically interrupted by a single task and then successfully continued.   rtos.c: Find a assembly fragment how to write pure assembly functions in order to circumvent the GCC bug with naked functions having local data in optimization level 0. See rtos.c, lines 712ff
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>Continuation of implementation rtos.c. First compilable revision, which is "running" with 0 tasks defined. No suspend operations so far</t>
+  </si>
+  <si>
+    <t>Continuation of implementation rtos.c. Implementation problems with first suspend operation; concept made but not proven or implemented yet</t>
+  </si>
+  <si>
+    <t>First suspend is running. TC02: Idle is periodically interrupted by a single task and then continued</t>
   </si>
 </sst>
 </file>
@@ -856,10 +862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -954,6 +960,31 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>41174</v>
+      </c>
+      <c r="B8">
+        <v>5.25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>41176</v>
+      </c>
+      <c r="B9">
+        <v>1.5</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
waitForEvent and setEvent completed. Herewith, the core code is basically implemented but not yet running. TC03 has been added which uses more than one task the very first time but the system crashes. No error investigation made yet
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>First suspend is running. TC02: Idle is periodically interrupted by a single task and then continued</t>
+  </si>
+  <si>
+    <t>waitForEvent, setEvent implemented. TC03 added, but does not yet run</t>
   </si>
 </sst>
 </file>
@@ -862,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -985,6 +988,25 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>41177</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>41178</v>
+      </c>
+      <c r="B11">
+        <v>2.5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
First non-trivial test cases are running well. Two or three tasks of same or shared priority are cycling well. rtos_delay is new and seems to work. setEvent is still missing and no inter-task communication has been tested so far.   GNUmakefile added which is intended to replace the dsmake make process soon. Not yet perfect, it is not possible to make build directory creation part of the rule hierarchy.   The dsmake makefile  solves a problem: Some of the ISRs (vectors) in HardwareSerial seem to use  12 Bit PC-relative jumps to get to their service routine. The branch distance is easily exceeded because the core.a is linked at the end - behind all of our code. Work around: All core.a files are linked as object files at the beginning. GNUmakefile doesn't have this work around so far
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="effort" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -43,13 +43,25 @@
     <t>Continuation of implementation rtos.c. First compilable revision, which is "running" with 0 tasks defined. No suspend operations so far</t>
   </si>
   <si>
-    <t>Continuation of implementation rtos.c. Implementation problems with first suspend operation; concept made but not proven or implemented yet</t>
-  </si>
-  <si>
     <t>First suspend is running. TC02: Idle is periodically interrupted by a single task and then continued</t>
   </si>
   <si>
     <t>waitForEvent, setEvent implemented. TC03 added, but does not yet run</t>
+  </si>
+  <si>
+    <t>Debugging of current implementation. Still no success with two tasks plus idle</t>
+  </si>
+  <si>
+    <t>First success with two tasks plus idle but not yet proven by profound testing</t>
+  </si>
+  <si>
+    <t>Specification of RTuinOS API</t>
+  </si>
+  <si>
+    <t>Continuation of implementation rtos.c. Implementation problems with first suspend operation; New implementation concept made but not proven or implemented yet</t>
+  </si>
+  <si>
+    <t>First non-trivial test cases are running well</t>
   </si>
 </sst>
 </file>
@@ -865,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -890,121 +902,168 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>41167</v>
-      </c>
-      <c r="B2">
-        <v>6</v>
+        <v>41164</v>
+      </c>
+      <c r="C2">
+        <v>2.5</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>41169</v>
+        <v>41167</v>
       </c>
       <c r="B3">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>41170</v>
+        <v>41169</v>
       </c>
       <c r="B4">
         <v>3.5</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>41171</v>
+        <v>41170</v>
       </c>
       <c r="B5">
+        <v>3.5</v>
+      </c>
+      <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>41172</v>
+        <v>41171</v>
       </c>
       <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>41173</v>
+        <v>41172</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>41174</v>
+        <v>41173</v>
       </c>
       <c r="B8">
-        <v>5.25</v>
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>41176</v>
+        <v>41174</v>
       </c>
       <c r="B9">
-        <v>1.5</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
+        <v>5.25</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>41177</v>
+        <v>41176</v>
+      </c>
+      <c r="B10">
+        <v>1.5</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
+        <v>41177</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>41178</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>2.5</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>41179</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>41180</v>
+      </c>
+      <c r="B14">
+        <v>3.75</v>
+      </c>
+      <c r="C14">
+        <v>0.25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>41183</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementation setEvent completed and integrated with onTimerTic. New, related test case 05 succeeds.   Starting point for doxygen documentation added
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>First non-trivial test cases are running well</t>
+  </si>
+  <si>
+    <t>Doxygen set up, setEvent completed and first related, new test case tc05 succeeds</t>
   </si>
 </sst>
 </file>
@@ -877,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1066,6 +1069,20 @@
         <v>15</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>41184</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>0.5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix: If a task has an overrun it must be made due again immediately. Before this fix, it had to wait for the system time to cycle around - which is actually a hanging task for system timers of >= 16 Bit.   Testing of setEvent/waitForEvent continued in tc05.   Implementation of task overrun counters and stack usage computation. Both tested a bit in tc05.   Implementation of application interrupts - however not yet tested at all. Can just be compiled
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>Doxygen set up, setEvent completed and first related, new test case tc05 succeeds</t>
+  </si>
+  <si>
+    <t>Implementation task overrun and stack usage, not tested yet</t>
+  </si>
+  <si>
+    <t>Implementation application interrupts, not tested yet. Testing of setEvent/waitForEvent</t>
   </si>
 </sst>
 </file>
@@ -880,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1074,13 +1080,38 @@
         <v>41184</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>0.5</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>41185</v>
+      </c>
+      <c r="B17">
+        <v>2.25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>41186</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Type rtos_task_t has been hidden, is now local to rtos.c.   All test case adapted to the changed style of task initialization. All test cases are compiling and running well.   This revision is a starting (and fall back) point for the intended re-implementation of the core - now using pointers to task objects instead of indexes
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Implementation application interrupts, not tested yet. Testing of setEvent/waitForEvent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code cleanup check of all test cases as preparation of re-implementation index-&gt;pointer </t>
   </si>
 </sst>
 </file>
@@ -886,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1114,6 +1117,17 @@
         <v>18</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>41187</v>
+      </c>
+      <c r="B19">
+        <v>1.75</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementation of round robin. The only test so far is tc06, a copy of tc05 with round robin activated. In this state tc06 just proves that rr can be compiled and doesn't crash.   Manual set up including the GNU Free Documentation License. The "notesForManual" have been copied into the empty document structure as only contents so far
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>Redesign of implementation of core using pointers to task objects</t>
+  </si>
+  <si>
+    <t>Implementation of Round-Robin. GNU FDL added to manual</t>
+  </si>
+  <si>
+    <t>Manual set up from LaTeX template</t>
   </si>
 </sst>
 </file>
@@ -892,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1142,6 +1148,28 @@
         <v>20</v>
       </c>
     </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>41190</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>41192</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix: The resume condition by events with a simple AND or OR was bad considering the timers: If all events are requested, the elapsed timer needs to be an exception: If it is seen, the task should immediately resume - otherwise it's no longer a timeout
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>Manual set up from LaTeX template</t>
+  </si>
+  <si>
+    <t>Manual continued</t>
+  </si>
+  <si>
+    <t>Fix: Bad specification of ALL events - now timer events are still an OR condition</t>
   </si>
 </sst>
 </file>
@@ -898,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1170,6 +1176,39 @@
         <v>21</v>
       </c>
     </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>41193</v>
+      </c>
+      <c r="B23">
+        <v>2.25</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>41194</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>41197</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Code cleanup. Comment code of former suspendTaskTillTime removed.   Task initialization now also supports absolute timer, behaves like waitForEvent.   Implementation of enterLeaveTask; still untested but can be compiled.   Only tc05 has been compiled and run
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -88,7 +88,10 @@
     <t>Manual continued</t>
   </si>
   <si>
-    <t>Fix: Bad specification of ALL events - now timer events are still an OR condition</t>
+    <t>Fix: Bad specification of ALL events - now timer events are still an OR condition. Implementation of waitForEventsTillTime by generalization of waitForEvent</t>
+  </si>
+  <si>
+    <t>Code cleanup, suspendTillTime discarded. Implementation of enter/leaveCriticalSection</t>
   </si>
 </sst>
 </file>
@@ -904,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1203,10 +1206,21 @@
         <v>41197</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="D25" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>41198</v>
+      </c>
+      <c r="B26">
+        <v>2.5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Manual continued. The abstract explanation of the fundamental concept of RTuinOS is completed
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -907,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1223,6 +1223,17 @@
         <v>25</v>
       </c>
     </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>41199</v>
+      </c>
+      <c r="B27">
+        <v>1.75</v>
+      </c>
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Manual continued. Chapter API completed as draft
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -907,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1234,6 +1234,28 @@
         <v>23</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>41200</v>
+      </c>
+      <c r="B28">
+        <v>1.75</v>
+      </c>
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>41205</v>
+      </c>
+      <c r="B29">
+        <v>2.5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Manual continued: Usage of Makefile completed as draft.   The folder sampleApp has been renamed to applications.   Some improvements of the makefile:   The name of the binaries now reflect which application has been compiled with RTuinOS.   Test case has been changed into app for application.   The help text has been revised and corrected.   The -I switches for the compiler are now computed from the source folder list. Double code could be removed
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -907,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1256,6 +1256,17 @@
         <v>23</v>
       </c>
     </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>41206</v>
+      </c>
+      <c r="B30">
+        <v>2.75</v>
+      </c>
+      <c r="D30" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Manual continued. System timer discussed.   Makefile: Dependency files included, manual adapted accordingly
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Code cleanup, suspendTillTime discarded. Implementation of enter/leaveCriticalSection</t>
+  </si>
+  <si>
+    <t>Makefile: Dependency files incorporated, Manual continued</t>
   </si>
 </sst>
 </file>
@@ -907,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1267,6 +1270,20 @@
         <v>23</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>41207</v>
+      </c>
+      <c r="B31">
+        <v>2.5</v>
+      </c>
+      <c r="C31">
+        <v>1.25</v>
+      </c>
+      <c r="D31" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Documentation improved of rtos.c and makefile.   Manual: First spelling check performed. Chapter Use Cases postponed, the rest is nearly completed in draft. Missing: Configuring application interrupts
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Makefile: Dependency files incorporated, Manual continued</t>
+  </si>
+  <si>
+    <t>Manual continued, widely completed as draft but without chapter Use Cases</t>
   </si>
 </sst>
 </file>
@@ -910,7 +913,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
@@ -1104,10 +1107,7 @@
         <v>41184</v>
       </c>
       <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>0.5</v>
+        <v>5.5</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
@@ -1282,6 +1282,17 @@
       </c>
       <c r="D31" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>41208</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Manual review completed, i.e. first "release" revision available.   Definition of timer tic macro moved to configuration template file as it depends on application customization of the timer interrupt.   All existing copies of the configuration file aligned with intermediate changes of the template (documentation and new macros)
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Manual continued, widely completed as draft but without chapter Use Cases</t>
+  </si>
+  <si>
+    <t>Manual reviewed</t>
   </si>
 </sst>
 </file>
@@ -913,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1295,6 +1298,42 @@
         <v>27</v>
       </c>
     </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>41212</v>
+      </c>
+      <c r="B33">
+        <v>2.75</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>41213</v>
+      </c>
+      <c r="B34">
+        <v>2.75</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>41214</v>
+      </c>
+      <c r="B35">
+        <v>1.5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New test case added. Test of critical sections and more tasks with more complex scheduling scheme. Implementation completed but never run so far.   Introductory section of manual revised, is probably okay now
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Manual reviewed</t>
+  </si>
+  <si>
+    <t>Manual continued, new test case tc07</t>
   </si>
 </sst>
 </file>
@@ -916,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1334,6 +1337,31 @@
         <v>28</v>
       </c>
     </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>41218</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>41219</v>
+      </c>
+      <c r="B37">
+        <v>1.75</v>
+      </c>
+      <c r="C37">
+        <v>0.25</v>
+      </c>
+      <c r="D37" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Creating script for installer started, is still widely incomplete.   New test case tc07 put to operation, succeeds.   Typos on other test cases
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Manual continued, new test case tc07</t>
+  </si>
+  <si>
+    <t>Creation of installer, test case tc07 put to operation</t>
   </si>
 </sst>
 </file>
@@ -919,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1362,6 +1365,20 @@
         <v>29</v>
       </c>
     </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>41220</v>
+      </c>
+      <c r="B38">
+        <v>2.25</v>
+      </c>
+      <c r="C38">
+        <v>0.75</v>
+      </c>
+      <c r="D38" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Documentation completed: readMe files for manual compilation and as entry point into documentation at installation time, doxygen rebuilt and put under source control, manual.pdf rebuilt and put under source control
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>Creation of installer, test case tc07 put to operation</t>
+  </si>
+  <si>
+    <t>Installer creation scripts continued, missing readMe files added</t>
   </si>
 </sst>
 </file>
@@ -922,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1379,6 +1382,17 @@
         <v>30</v>
       </c>
     </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>41221</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New test case tc08 for application interrupts added. Implementation widely done but all hardware related interrupt settings are still missing (enableIsr, enter/leaveCriticalSection).   The dependent documentation files are taken out of source control as they are now compiled as part of the setup creation process.   Startup message unified.   An obsolete comment removed from most test case implementation files
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Installer creation scripts continued, missing readMe files added</t>
+  </si>
+  <si>
+    <t>Installer creation scripts continued, new test case tc08</t>
   </si>
 </sst>
 </file>
@@ -925,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1393,6 +1396,17 @@
         <v>31</v>
       </c>
     </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>41225</v>
+      </c>
+      <c r="B40">
+        <v>3.5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix: The application interrupt service routines didn't clear the zero register before jumping into the compiler generated code. This caused occasional bad return values of the suspend command, seen as phantom timeout events in the application. Test case tc08 succeeds now
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>Installer creation scripts continued, new test case tc08</t>
+  </si>
+  <si>
+    <t>Test case tc08 put to operation but still shows some bad behavior</t>
   </si>
 </sst>
 </file>
@@ -928,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1097,10 +1100,7 @@
         <v>41180</v>
       </c>
       <c r="B14">
-        <v>3.75</v>
-      </c>
-      <c r="C14">
-        <v>0.25</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
@@ -1362,10 +1362,7 @@
         <v>41219</v>
       </c>
       <c r="B37">
-        <v>1.75</v>
-      </c>
-      <c r="C37">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="D37" t="s">
         <v>29</v>
@@ -1405,6 +1402,17 @@
       </c>
       <c r="D40" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>41227</v>
+      </c>
+      <c r="B41">
+        <v>2.5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: Build process of Arduino limited program size to a few kByte because of bad usage of short jumps in the vector table
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t>Test case tc08 put to operation but still shows some bad behavior</t>
+  </si>
+  <si>
+    <t>Test case tc08 is working well, a fix of rtos.c was required. All test cases rerun. Manual updated</t>
+  </si>
+  <si>
+    <t>Preparation of release, new test case tc09</t>
+  </si>
+  <si>
+    <t>Makefile: Workaround for 12 Bit Branch distance problem with core.a</t>
   </si>
 </sst>
 </file>
@@ -931,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1415,6 +1424,39 @@
         <v>33</v>
       </c>
     </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>41228</v>
+      </c>
+      <c r="B42">
+        <v>2.5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>41229</v>
+      </c>
+      <c r="B43">
+        <v>3.25</v>
+      </c>
+      <c r="D43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>41232</v>
+      </c>
+      <c r="B44">
+        <v>1.25</v>
+      </c>
+      <c r="D44" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
tc09 completed. Pseudo mutex now implemented with event on release
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>Makefile: Workaround for 12 Bit Branch distance problem with core.a</t>
+  </si>
+  <si>
+    <t>New test case tc09 put to operation and completed. Fix of makefile. Documentation. Export for Andreas</t>
   </si>
 </sst>
 </file>
@@ -940,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1457,6 +1460,17 @@
         <v>36</v>
       </c>
     </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>41233</v>
+      </c>
+      <c r="B45">
+        <v>2.5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Minor changes on documentation and setup.   rtos_enter/leaveCriticalSection of tc08 aligned with standard implementation
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>New test case tc09 put to operation and completed. Fix of makefile. Documentation. Export for Andreas</t>
+  </si>
+  <si>
+    <t>Minor changes on documentation and setup</t>
   </si>
 </sst>
 </file>
@@ -943,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1471,6 +1474,17 @@
         <v>37</v>
       </c>
     </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>41234</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
tc10 added, which introduces and validates a simple system load estimation
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Date</t>
   </si>
@@ -131,6 +131,15 @@
   </si>
   <si>
     <t>Minor changes on documentation and setup</t>
+  </si>
+  <si>
+    <t>System load estimation</t>
+  </si>
+  <si>
+    <t>Minor changes on documentation and setup. System load estimation</t>
+  </si>
+  <si>
+    <t>tc: System load estimation put to operation, validated by test case tc10</t>
   </si>
 </sst>
 </file>
@@ -946,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1485,6 +1494,39 @@
         <v>38</v>
       </c>
     </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>41239</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="D47" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>41241</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>41242</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="D49" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
tc05: Timeout condition made much sharper.   tc10: Documention completed   doxygen documentation reviewed in parts
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -136,10 +136,13 @@
     <t>System load estimation</t>
   </si>
   <si>
-    <t>Minor changes on documentation and setup. System load estimation</t>
-  </si>
-  <si>
     <t>tc: System load estimation put to operation, validated by test case tc10</t>
+  </si>
+  <si>
+    <t>tc05 revised, documentation of rtos.c/h extended/corrected</t>
+  </si>
+  <si>
+    <t>Documentation, tc10 and doxygen</t>
   </si>
 </sst>
 </file>
@@ -955,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1499,10 +1502,10 @@
         <v>41239</v>
       </c>
       <c r="B47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1524,7 +1527,29 @@
         <v>2</v>
       </c>
       <c r="D49" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>41243</v>
+      </c>
+      <c r="B50">
+        <v>3.75</v>
+      </c>
+      <c r="D50" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>41244</v>
+      </c>
+      <c r="B51">
+        <v>1.75</v>
+      </c>
+      <c r="D51" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Manual: New Section Task Switches. The general story, which does not yet explain the specifics of RTuinOS
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Documentation, tc10 and doxygen</t>
+  </si>
+  <si>
+    <t>Manual: New section "Task switches" started</t>
   </si>
 </sst>
 </file>
@@ -958,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1552,6 +1555,17 @@
         <v>42</v>
       </c>
     </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>41246</v>
+      </c>
+      <c r="B52">
+        <v>2.5</v>
+      </c>
+      <c r="D52" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Manual: New section 2.7, implementation of task switches completed and reviewed.   Discussion of data type of system time, 4.4., written completely new. Not yet read/reviewed
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t>Manual: New section "Task switches" started</t>
+  </si>
+  <si>
+    <t>Manual: new section continued, new figure for illustration</t>
+  </si>
+  <si>
+    <t>Manual: new section 2.7 completed, including new figures and first review</t>
+  </si>
+  <si>
+    <t>Manual: Section 4.4, data type system time rewritten</t>
   </si>
 </sst>
 </file>
@@ -961,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1566,6 +1575,42 @@
         <v>43</v>
       </c>
     </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>41247</v>
+      </c>
+      <c r="B53">
+        <v>2.5</v>
+      </c>
+      <c r="D53" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>41248</v>
+      </c>
+      <c r="B54">
+        <v>0.75</v>
+      </c>
+      <c r="C54">
+        <v>2.5</v>
+      </c>
+      <c r="D54" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>41249</v>
+      </c>
+      <c r="B55">
+        <v>2.5</v>
+      </c>
+      <c r="D55" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
2nd review of manual completed
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>Manual: Section 4.4, data type system time rewritten</t>
+  </si>
+  <si>
+    <t>Manual: 2nd review completed</t>
+  </si>
+  <si>
+    <t>Manual: 2nd review continued</t>
   </si>
 </sst>
 </file>
@@ -970,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1611,6 +1617,28 @@
         <v>46</v>
       </c>
     </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>41254</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>41255</v>
+      </c>
+      <c r="B57">
+        <v>1.75</v>
+      </c>
+      <c r="D57" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Preparation of release: Last changes on documentation.   Fix: Setup creation disregarded graphics file format *.png
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>Date</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>Manual: 2nd review continued</t>
+  </si>
+  <si>
+    <t>Documentation of code slightly improved</t>
   </si>
 </sst>
 </file>
@@ -976,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1360,10 +1363,7 @@
         <v>41212</v>
       </c>
       <c r="B33">
-        <v>2.75</v>
-      </c>
-      <c r="C33">
-        <v>2</v>
+        <v>4.75</v>
       </c>
       <c r="D33" t="s">
         <v>23</v>
@@ -1637,6 +1637,17 @@
       </c>
       <c r="D57" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>41256</v>
+      </c>
+      <c r="B58">
+        <v>0.5</v>
+      </c>
+      <c r="D58" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Effort calculation updated.   Minor documentation changes
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -981,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1006,7 +1006,7 @@
       <c r="A2" s="1">
         <v>41164</v>
       </c>
-      <c r="C2">
+      <c r="B2">
         <v>2.5</v>
       </c>
       <c r="D2" t="s">
@@ -1040,10 +1040,7 @@
         <v>41170</v>
       </c>
       <c r="B5">
-        <v>3.5</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
+        <v>5.5</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -1338,10 +1335,10 @@
         <v>41207</v>
       </c>
       <c r="B31">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="C31">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="D31" t="s">
         <v>26</v>
@@ -1418,10 +1415,7 @@
         <v>41220</v>
       </c>
       <c r="B38">
-        <v>2.25</v>
-      </c>
-      <c r="C38">
-        <v>0.75</v>
+        <v>3</v>
       </c>
       <c r="D38" t="s">
         <v>30</v>
@@ -1597,10 +1591,7 @@
         <v>41248</v>
       </c>
       <c r="B54">
-        <v>0.75</v>
-      </c>
-      <c r="C54">
-        <v>2.5</v>
+        <v>3.25</v>
       </c>
       <c r="D54" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Account balance, column additional effort removed
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
   <si>
     <t>Effort [h]</t>
-  </si>
-  <si>
-    <t>Additional Effort [h]</t>
   </si>
   <si>
     <t>C code of scheduler core</t>
@@ -979,666 +976,646 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="72.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>41164</v>
       </c>
       <c r="B2">
         <v>2.5</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>41167</v>
       </c>
       <c r="B3">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>41169</v>
       </c>
       <c r="B4">
         <v>3.5</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>41170</v>
       </c>
       <c r="B5">
         <v>5.5</v>
       </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>41171</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>41172</v>
       </c>
       <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>41173</v>
       </c>
       <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>41174</v>
       </c>
       <c r="B9">
         <v>5.25</v>
       </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>41176</v>
       </c>
       <c r="B10">
-        <v>1.5</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>41177</v>
       </c>
-      <c r="C11">
+      <c r="B11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>41178</v>
       </c>
       <c r="B12">
         <v>2.5</v>
       </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>41179</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>41180</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>41183</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>41184</v>
       </c>
       <c r="B16">
         <v>5.5</v>
       </c>
-      <c r="D16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>41185</v>
       </c>
       <c r="B17">
         <v>2.25</v>
       </c>
-      <c r="D17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>41186</v>
       </c>
       <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>41187</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
-      <c r="D19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>41188</v>
       </c>
       <c r="B20">
         <v>3.25</v>
       </c>
-      <c r="D20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>41190</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="D21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>41192</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
-      <c r="D22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>41193</v>
       </c>
       <c r="B23">
         <v>2.25</v>
       </c>
-      <c r="D23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>41194</v>
       </c>
       <c r="B24">
         <v>5</v>
       </c>
-      <c r="D24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>41197</v>
       </c>
       <c r="B25">
         <v>2.5</v>
       </c>
-      <c r="D25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>41198</v>
       </c>
       <c r="B26">
         <v>2.5</v>
       </c>
-      <c r="D26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>41199</v>
       </c>
       <c r="B27">
         <v>1.75</v>
       </c>
-      <c r="D27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>41200</v>
       </c>
       <c r="B28">
         <v>1.75</v>
       </c>
-      <c r="D28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>41205</v>
       </c>
       <c r="B29">
         <v>2.5</v>
       </c>
-      <c r="D29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>41206</v>
       </c>
       <c r="B30">
         <v>2.75</v>
       </c>
-      <c r="D30" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>41207</v>
       </c>
       <c r="B31">
-        <v>2.75</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3.75</v>
+      </c>
+      <c r="C31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>41208</v>
       </c>
       <c r="B32">
         <v>4</v>
       </c>
-      <c r="D32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>41212</v>
       </c>
       <c r="B33">
         <v>4.75</v>
       </c>
-      <c r="D33" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>41213</v>
       </c>
       <c r="B34">
         <v>2.75</v>
       </c>
-      <c r="D34" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>41214</v>
       </c>
       <c r="B35">
         <v>1.5</v>
       </c>
-      <c r="D35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>41218</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-      <c r="D36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>41219</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
-      <c r="D37" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>41220</v>
       </c>
       <c r="B38">
         <v>3</v>
       </c>
-      <c r="D38" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>41221</v>
       </c>
       <c r="B39">
         <v>3</v>
       </c>
-      <c r="D39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>41225</v>
       </c>
       <c r="B40">
         <v>3.5</v>
       </c>
-      <c r="D40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>41227</v>
       </c>
       <c r="B41">
         <v>2.5</v>
       </c>
-      <c r="D41" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41228</v>
       </c>
       <c r="B42">
         <v>2.5</v>
       </c>
-      <c r="D42" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41229</v>
       </c>
       <c r="B43">
         <v>3.25</v>
       </c>
-      <c r="D43" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>41232</v>
       </c>
       <c r="B44">
         <v>1.25</v>
       </c>
-      <c r="D44" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>41233</v>
       </c>
       <c r="B45">
         <v>2.5</v>
       </c>
-      <c r="D45" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>41234</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
-      <c r="D46" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>41239</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
-      <c r="D47" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>41241</v>
       </c>
       <c r="B48">
         <v>2</v>
       </c>
-      <c r="D48" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>41242</v>
       </c>
       <c r="B49">
         <v>2</v>
       </c>
-      <c r="D49" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>41243</v>
       </c>
       <c r="B50">
         <v>3.75</v>
       </c>
-      <c r="D50" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>41244</v>
       </c>
       <c r="B51">
         <v>1.75</v>
       </c>
-      <c r="D51" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>41246</v>
       </c>
       <c r="B52">
         <v>2.5</v>
       </c>
-      <c r="D52" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>41247</v>
       </c>
       <c r="B53">
         <v>2.5</v>
       </c>
-      <c r="D53" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>41248</v>
       </c>
       <c r="B54">
         <v>3.25</v>
       </c>
-      <c r="D54" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>41249</v>
       </c>
       <c r="B55">
         <v>2.5</v>
       </c>
-      <c r="D55" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>41254</v>
       </c>
       <c r="B56">
         <v>1</v>
       </c>
-      <c r="D56" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>41255</v>
       </c>
       <c r="B57">
         <v>1.75</v>
       </c>
-      <c r="D57" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C57" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>41256</v>
       </c>
       <c r="B58">
         <v>0.5</v>
       </c>
-      <c r="D58" t="s">
-        <v>49</v>
+      <c r="C58" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleanup of code (@todo tags reviewed) of RTuinOS and test cases.   RTuinOS startup message made available in flash ROM. New convenience function puts_progmem offered (via test case code) to use such cheap, constant strings
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Successful completion of tc13</t>
+  </si>
+  <si>
+    <t>Unsuccessful, reverted attempt to optimize context switch code</t>
   </si>
 </sst>
 </file>
@@ -1022,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1248,6 +1251,28 @@
       </c>
       <c r="D18" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>41449</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>41450</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Very early state of tc14 put under source control. ADC is running well, input and reference voltage can be selected, but no task is applied or configured so far
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
   <si>
     <t>Date</t>
   </si>
@@ -210,6 +210,15 @@
   </si>
   <si>
     <t>Unsuccessful, reverted attempt to optimize context switch code</t>
+  </si>
+  <si>
+    <t>TODOs, code cleanup</t>
+  </si>
+  <si>
+    <t>Concept of tc14</t>
+  </si>
+  <si>
+    <t>Implementation tc14</t>
   </si>
 </sst>
 </file>
@@ -1025,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1172,10 +1181,10 @@
         <v>41439</v>
       </c>
       <c r="B12">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
         <v>59</v>
@@ -1246,7 +1255,7 @@
       <c r="A18" s="1">
         <v>41446</v>
       </c>
-      <c r="C18">
+      <c r="B18">
         <v>2.25</v>
       </c>
       <c r="D18" t="s">
@@ -1273,6 +1282,39 @@
       </c>
       <c r="D20" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>41452</v>
+      </c>
+      <c r="B21">
+        <v>2.5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>41455</v>
+      </c>
+      <c r="B22">
+        <v>1.5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>41456</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: Missing file added   Documentary changes
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
   <si>
     <t>Date</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>Implementation tc14</t>
+  </si>
+  <si>
+    <t>Implementation tc14, variants tried</t>
   </si>
 </sst>
 </file>
@@ -1034,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1315,6 +1318,17 @@
       </c>
       <c r="D23" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>41457</v>
+      </c>
+      <c r="B24">
+        <v>2.5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sudar Muthu: Linus support requires case sensitive file name. arduino.h changed in Arduino.h
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Implementation tc14, variants tried</t>
+  </si>
+  <si>
+    <t>SVN branch: gcc versus g++. Revision of Makefile, support of Linux and Windows, modularization</t>
   </si>
 </sst>
 </file>
@@ -1037,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1220,10 +1223,7 @@
         <v>41443</v>
       </c>
       <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
         <v>60</v>
@@ -1234,10 +1234,10 @@
         <v>41444</v>
       </c>
       <c r="B16">
-        <v>1.5</v>
+        <v>2.75</v>
       </c>
       <c r="C16">
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
       <c r="D16" t="s">
         <v>61</v>
@@ -1329,6 +1329,17 @@
       </c>
       <c r="D24" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>41462</v>
+      </c>
+      <c r="B25">
+        <v>2.5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Makefile: Callback into application to support application specific settings.   tc14: Implementation continued. Now using LCD shield to display ADC measurement results. Still not complete, input selection by buttons is not yet done
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
   <si>
     <t>Date</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>SVN branch: gcc versus g++. Revision of Makefile, support of Linux and Windows, modularization</t>
+  </si>
+  <si>
+    <t>Revision manual</t>
   </si>
 </sst>
 </file>
@@ -1040,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1333,13 +1336,57 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
+        <v>41458</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>41461</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>41462</v>
       </c>
-      <c r="B25">
+      <c r="B27">
         <v>2.5</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D27" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>41463</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>41464</v>
+      </c>
+      <c r="B29">
+        <v>1.5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tc14: Additional, independent task designed, which implements a real time clock. Source folder structure shaped to demonstrate the use of the makefile "callback".   Manual: Figure extended and typo corrected.
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Effort R 1.0" sheetId="3" r:id="rId1"/>
     <sheet name="Effort R 0.9" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
   <si>
     <t>Date</t>
   </si>
@@ -170,12 +170,6 @@
     <t>Task</t>
   </si>
   <si>
-    <t>Revision of Makefile</t>
-  </si>
-  <si>
-    <t>Documentation Makefile changes. Concept for new sync objects</t>
-  </si>
-  <si>
     <t>Concept of new sync objects</t>
   </si>
   <si>
@@ -228,6 +222,12 @@
   </si>
   <si>
     <t>Revision manual</t>
+  </si>
+  <si>
+    <t>Revision of makefile</t>
+  </si>
+  <si>
+    <t>Documentation makefile changes. Concept for new sync objects</t>
   </si>
 </sst>
 </file>
@@ -1043,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1080,7 +1080,7 @@
         <v>2.5</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1091,7 +1091,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1102,7 +1102,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1113,7 +1113,7 @@
         <v>0.75</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1124,7 +1124,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1135,7 +1135,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1149,7 +1149,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1160,7 +1160,7 @@
         <v>2.25</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1171,7 +1171,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1182,7 +1182,7 @@
         <v>1.5</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1196,7 +1196,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1207,7 +1207,7 @@
         <v>2.5</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1218,7 +1218,7 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1229,7 +1229,7 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1243,7 +1243,7 @@
         <v>1.25</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1254,7 +1254,7 @@
         <v>0.5</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1265,7 +1265,7 @@
         <v>2.25</v>
       </c>
       <c r="D18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1276,7 +1276,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1287,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1298,7 +1298,7 @@
         <v>2.5</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1309,7 +1309,7 @@
         <v>1.5</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1320,7 +1320,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1331,7 +1331,7 @@
         <v>2.5</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1342,7 +1342,7 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1353,7 +1353,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1364,7 +1364,7 @@
         <v>2.5</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1374,8 +1374,11 @@
       <c r="B28">
         <v>2</v>
       </c>
+      <c r="C28">
+        <v>0.25</v>
+      </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1386,7 +1389,18 @@
         <v>1.5</v>
       </c>
       <c r="D29" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>41465</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tc14 is now complete and successfully running. Documentation is not yet completed
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Effort R 1.0" sheetId="3" r:id="rId1"/>
     <sheet name="Effort R 0.9" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
   <si>
     <t>Date</t>
   </si>
@@ -1043,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1400,6 +1400,31 @@
         <v>2</v>
       </c>
       <c r="D30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>41466</v>
+      </c>
+      <c r="B31">
+        <v>2.5</v>
+      </c>
+      <c r="C31">
+        <v>1.5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>41467</v>
+      </c>
+      <c r="C32">
+        <v>4.25</v>
+      </c>
+      <c r="D32" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Main application file with with completed documentation of the test case moved to the application root where one would expect to find some introductory text
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>Documentation makefile changes. Concept for new sync objects</t>
+  </si>
+  <si>
+    <t>Implementation and documentation of tc14</t>
   </si>
 </sst>
 </file>
@@ -1045,9 +1048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1421,11 +1422,14 @@
       <c r="A32" s="1">
         <v>41467</v>
       </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
       <c r="C32">
         <v>4.25</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Many review comments of manual incorporated into LaTeX sources
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t>All test cases run; many typos/correction in the test case documentation</t>
+  </si>
+  <si>
+    <t>Setup creation, prerelease sent to Sudar Muthu</t>
+  </si>
+  <si>
+    <t>Revision of manual</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1446,6 +1452,28 @@
       </c>
       <c r="D33" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>41471</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>41472</v>
+      </c>
+      <c r="B35">
+        <v>1.25</v>
+      </c>
+      <c r="D35" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Manual renamed to User Guide.   Comments of review incorporated
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -233,13 +233,13 @@
     <t>Implementation and documentation of tc14</t>
   </si>
   <si>
+    <t>Setup creation, prerelease sent to Sudar Muthu</t>
+  </si>
+  <si>
+    <t>Revision of manual</t>
+  </si>
+  <si>
     <t>All test cases run; many typos/correction in the test case documentation</t>
-  </si>
-  <si>
-    <t>Setup creation, prerelease sent to Sudar Muthu</t>
-  </si>
-  <si>
-    <t>Revision of manual</t>
   </si>
 </sst>
 </file>
@@ -1055,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1451,7 +1451,7 @@
         <v>2.5</v>
       </c>
       <c r="D33" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1461,8 +1461,11 @@
       <c r="B34">
         <v>1</v>
       </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
       <c r="D34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1473,7 +1476,18 @@
         <v>1.25</v>
       </c>
       <c r="D35" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>41473</v>
+      </c>
+      <c r="B36">
+        <v>1.5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revision of test case tc06
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
   <si>
     <t>Date</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>Refactoring: posting events and code review, tests re-run, boolean_t, sendEvent</t>
+  </si>
+  <si>
+    <t>Revision of tc06</t>
   </si>
 </sst>
 </file>
@@ -1064,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1541,6 +1544,17 @@
       </c>
       <c r="D40" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>41480</v>
+      </c>
+      <c r="B41">
+        <v>2.5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Review comments on manual completely integrated into LaTeX source files
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
   <si>
     <t>Date</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>Revision of tc06</t>
+  </si>
+  <si>
+    <t>Revision of manual completed</t>
   </si>
 </sst>
 </file>
@@ -1067,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1555,6 +1558,17 @@
       </c>
       <c r="D41" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>41481</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New typedef boolean_t removed again to be closer to Arduino (and share the inconsistency in naming with it).   stdout: Two versions did exist, only one supported puts_progmem. Equalized
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
   <si>
     <t>Date</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>Revision of manual completed</t>
+  </si>
+  <si>
+    <t>New test case tc15 implemented</t>
   </si>
 </sst>
 </file>
@@ -1070,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1569,6 +1572,17 @@
       </c>
       <c r="D42" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>41482</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="D43" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Typos in config template distributed into all application config's.   rtos.h: Definition of names of general purpose events extended to support a variable number of mutexes in case of use/non use of application interrupts
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -1082,7 +1082,7 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1605,6 +1605,9 @@
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>41485</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
       </c>
       <c r="C45">
         <v>1.5</v>

</xml_diff>

<commit_message>
rtos.h: new #define to hide the use of __attribute__ for the definition of the RTuinOS startup message in flash ROM.   Many minor documentary changes, mostly typos
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.xlsx
+++ b/RTuinOS/doc/effort.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="84">
   <si>
     <t>Date</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>Documentation test case tc12; re-integration of Sudars comments of July 29 into the code</t>
+  </si>
+  <si>
+    <t>Preparation of setup and release</t>
   </si>
 </sst>
 </file>
@@ -1079,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1408,10 +1411,7 @@
         <v>41463</v>
       </c>
       <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28">
-        <v>0.25</v>
+        <v>2.25</v>
       </c>
       <c r="D28" t="s">
         <v>68</v>
@@ -1444,10 +1444,7 @@
         <v>41466</v>
       </c>
       <c r="B31">
-        <v>2.5</v>
-      </c>
-      <c r="C31">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="D31" t="s">
         <v>65</v>
@@ -1614,6 +1611,28 @@
       </c>
       <c r="D45" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>41486</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>41489</v>
+      </c>
+      <c r="B47">
+        <v>1.5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1627,7 +1646,7 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>